<commit_message>
Cambiar excel por archivo previo
</commit_message>
<xml_diff>
--- a/assets/Plantilla_Lista_de_cargas.xlsx
+++ b/assets/Plantilla_Lista_de_cargas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive\Desktop\2025-2\Fotovoltaica\Aplicacion LDC\gustavo\proyecto-ldc\proyecto-ldc\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A8A53C-D8BA-4D3C-AE8B-D221B4ADDB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B332B10-1203-4845-938C-B1C6F1476818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>Carga 29</t>
   </si>
   <si>
-    <t>dada</t>
-  </si>
-  <si>
     <t>Carga 1</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>Carga 5</t>
+  </si>
+  <si>
+    <t>Carga 30</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
   <dimension ref="A1:AA31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -782,11 +782,9 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1">
         <v>0</v>
       </c>
@@ -803,16 +801,16 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
@@ -827,19 +825,19 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" s="1">
         <v>0</v>
@@ -865,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -948,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -1031,7 +1029,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -1114,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -3181,7 +3179,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>

</xml_diff>